<commit_message>
Updates with 6/24 release
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21225" windowHeight="9975"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21225" windowHeight="9975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="14" r:id="rId1"/>
@@ -216,7 +216,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=1065</stp>
+        <stp>cols=2;rows=1066</stp>
         <tr r="A5" s="7"/>
       </tp>
       <tp>
@@ -231,7 +231,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=1065</stp>
+        <stp>cols=2;rows=1066</stp>
         <tr r="A5" s="6"/>
       </tp>
       <tp>
@@ -246,7 +246,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=1065</stp>
+        <stp>cols=2;rows=1066</stp>
         <tr r="A5" s="5"/>
       </tp>
       <tp>
@@ -261,7 +261,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=1065</stp>
+        <stp>cols=2;rows=1066</stp>
         <tr r="A5" s="12"/>
       </tp>
       <tp>
@@ -276,7 +276,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=1065</stp>
+        <stp>cols=2;rows=1066</stp>
         <tr r="A5" s="13"/>
       </tp>
       <tp>
@@ -291,7 +291,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=1065</stp>
+        <stp>cols=2;rows=1066</stp>
         <tr r="A5" s="3"/>
       </tp>
       <tp t="s">
@@ -303,8 +303,6 @@
         <stp>[data.xlsx]key!R12C2</stp>
         <tr r="B12" s="14"/>
       </tp>
-    </main>
-    <main first="bloomberg.rtd">
       <tp t="s">
         <v>Persons Claiming Emergency Unemployment Compensation Benefits</v>
         <stp/>
@@ -331,6 +329,21 @@
         <stp>LONG_COMP_NAME</stp>
         <stp>[data.xlsx]key!R13C2</stp>
         <tr r="B13" s="14"/>
+      </tp>
+      <tp>
+        <v>43938</v>
+        <stp/>
+        <stp>##V3_BDHV12</stp>
+        <stp>INJCPUA Index</stp>
+        <stp>PX_LAST</stp>
+        <stp>1/1/2000</stp>
+        <stp/>
+        <stp>[data.xlsx]injcpua!R5C1</stp>
+        <stp>Dir=V</stp>
+        <stp>Per=W</stp>
+        <stp>Dts=S</stp>
+        <stp>cols=2;rows=10</stp>
+        <tr r="A5" s="2"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -375,7 +388,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=1067</stp>
+        <stp>cols=2;rows=1068</stp>
         <tr r="A5" s="1"/>
       </tp>
       <tp t="s">
@@ -387,8 +400,6 @@
         <stp>[data.xlsx]key!R4C2</stp>
         <tr r="B4" s="14"/>
       </tp>
-    </main>
-    <main first="bloomberg.rtd">
       <tp>
         <v>36532</v>
         <stp/>
@@ -401,7 +412,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=1065</stp>
+        <stp>cols=2;rows=1066</stp>
         <tr r="A5" s="11"/>
       </tp>
       <tp t="s">
@@ -438,21 +449,6 @@
         <tr r="A5" s="10"/>
       </tp>
       <tp>
-        <v>43938</v>
-        <stp/>
-        <stp>##V3_BDHV12</stp>
-        <stp>INJCPUA Index</stp>
-        <stp>PX_LAST</stp>
-        <stp>1/1/2000</stp>
-        <stp/>
-        <stp>[data.xlsx]injcpua!R5C1</stp>
-        <stp>Dir=V</stp>
-        <stp>Per=W</stp>
-        <stp>Dts=S</stp>
-        <stp>cols=2;rows=9</stp>
-        <tr r="A5" s="2"/>
-      </tp>
-      <tp>
         <v>43931</v>
         <stp/>
         <stp>##V3_BDHV12</stp>
@@ -464,7 +460,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=8</stp>
+        <stp>cols=2;rows=9</stp>
         <tr r="A5" s="8"/>
       </tp>
       <tp>
@@ -479,7 +475,7 @@
         <stp>Dir=V</stp>
         <stp>Per=W</stp>
         <stp>Dts=S</stp>
-        <stp>cols=2;rows=8</stp>
+        <stp>cols=2;rows=9</stp>
         <tr r="A5" s="9"/>
       </tp>
       <tp t="s">
@@ -491,8 +487,6 @@
         <stp>[data.xlsx]key!R3C2</stp>
         <tr r="B3" s="14"/>
       </tp>
-    </main>
-    <main first="bloomberg.rtd">
       <tp t="s">
         <v>US Initial Jobless Claims SA</v>
         <stp/>
@@ -772,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -7798,7 +7792,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1069"/>
+  <dimension ref="A1:D1070"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -7832,7 +7826,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1065")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1066")</f>
         <v>36532</v>
       </c>
       <c r="B5">
@@ -16332,7 +16326,7 @@
         <v>43966</v>
       </c>
       <c r="B1067">
-        <v>1.3820000000000001</v>
+        <v>1.381</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.25">
@@ -16349,6 +16343,14 @@
       </c>
       <c r="B1069">
         <v>2.7109999999999999</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B1070">
+        <v>2.98</v>
       </c>
     </row>
   </sheetData>
@@ -16361,7 +16363,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1069"/>
+  <dimension ref="A1:D1070"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -16395,7 +16397,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1065")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1066")</f>
         <v>36532</v>
       </c>
       <c r="B5">
@@ -24912,6 +24914,14 @@
       </c>
       <c r="B1069">
         <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B1070">
+        <v>2.4</v>
       </c>
     </row>
   </sheetData>
@@ -24924,7 +24934,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1069"/>
+  <dimension ref="A1:D1070"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -24958,7 +24968,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1065")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1066")</f>
         <v>36532</v>
       </c>
       <c r="B5">
@@ -33450,7 +33460,7 @@
         <v>43959</v>
       </c>
       <c r="B1066">
-        <v>178.92</v>
+        <v>178.88</v>
       </c>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.25">
@@ -33475,6 +33485,14 @@
       </c>
       <c r="B1069">
         <v>226.86</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B1070">
+        <v>292.08</v>
       </c>
     </row>
   </sheetData>
@@ -33487,9 +33505,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1071"/>
+  <dimension ref="A1:D1072"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1063" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -33525,7 +33543,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1067")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1068")</f>
         <v>36532</v>
       </c>
       <c r="B5">
@@ -42057,7 +42075,15 @@
         <v>43994</v>
       </c>
       <c r="B1071">
-        <v>1508</v>
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1072" s="1">
+        <v>44001</v>
+      </c>
+      <c r="B1072">
+        <v>1480</v>
       </c>
     </row>
   </sheetData>
@@ -42070,7 +42096,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -42107,7 +42133,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=9")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=10")</f>
         <v>43938</v>
       </c>
       <c r="B5">
@@ -42167,7 +42193,7 @@
         <v>43987</v>
       </c>
       <c r="B12">
-        <v>694.46299999999997</v>
+        <v>700.39300000000003</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -42175,7 +42201,15 @@
         <v>43994</v>
       </c>
       <c r="B13">
-        <v>760.52599999999995</v>
+        <v>770.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44001</v>
+      </c>
+      <c r="B14">
+        <v>728.12</v>
       </c>
     </row>
   </sheetData>
@@ -42188,7 +42222,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1069"/>
+  <dimension ref="A1:D1070"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -42222,7 +42256,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1065")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1066")</f>
         <v>36532</v>
       </c>
       <c r="B5">
@@ -50714,7 +50748,7 @@
         <v>43959</v>
       </c>
       <c r="B1066">
-        <v>30957.16</v>
+        <v>30957.119999999999</v>
       </c>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.25">
@@ -50722,7 +50756,7 @@
         <v>43966</v>
       </c>
       <c r="B1067">
-        <v>30167.17</v>
+        <v>29965.42</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.25">
@@ -50730,7 +50764,7 @@
         <v>43973</v>
       </c>
       <c r="B1068">
-        <v>29516.080000000002</v>
+        <v>29505.06</v>
       </c>
     </row>
     <row r="1069" spans="1:2" x14ac:dyDescent="0.25">
@@ -50738,7 +50772,15 @@
         <v>43980</v>
       </c>
       <c r="B1069">
-        <v>29165.75</v>
+        <v>29259.51</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B1070">
+        <v>30553.82</v>
       </c>
     </row>
   </sheetData>
@@ -50751,7 +50793,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1069"/>
+  <dimension ref="A1:D1070"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -50785,7 +50827,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1065")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1066")</f>
         <v>36532</v>
       </c>
       <c r="B5">
@@ -59285,7 +59327,7 @@
         <v>43966</v>
       </c>
       <c r="B1067">
-        <v>18791.93</v>
+        <v>18788.63</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.25">
@@ -59301,7 +59343,15 @@
         <v>43980</v>
       </c>
       <c r="B1069">
-        <v>18548.29</v>
+        <v>18548.439999999999</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B1070">
+        <v>18330.150000000001</v>
       </c>
     </row>
   </sheetData>
@@ -59314,7 +59364,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1069"/>
+  <dimension ref="A1:D1070"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -59348,7 +59398,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1065")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1066")</f>
         <v>36532</v>
       </c>
       <c r="B5">
@@ -67848,7 +67898,7 @@
         <v>43966</v>
       </c>
       <c r="B1067">
-        <v>14.848000000000001</v>
+        <v>14.856</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.25">
@@ -67865,6 +67915,14 @@
       </c>
       <c r="B1069">
         <v>15.513999999999999</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B1070">
+        <v>15.339</v>
       </c>
     </row>
   </sheetData>
@@ -67877,7 +67935,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1069"/>
+  <dimension ref="A1:D1070"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -67911,7 +67969,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1065")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=1066")</f>
         <v>36532</v>
       </c>
       <c r="B5">
@@ -76411,7 +76469,7 @@
         <v>43966</v>
       </c>
       <c r="B1067">
-        <v>11.39</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.25">
@@ -76428,6 +76486,14 @@
       </c>
       <c r="B1069">
         <v>11.9</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B1070">
+        <v>12.48</v>
       </c>
     </row>
   </sheetData>
@@ -76474,7 +76540,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=8")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=9")</f>
         <v>43931</v>
       </c>
       <c r="B5">
@@ -76534,11 +76600,16 @@
         <v>43980</v>
       </c>
       <c r="B12">
-        <v>9280.6440000000002</v>
+        <v>9374.2479999999996</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B13">
+        <v>11046.401</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -79752,7 +79823,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=8")</f>
+        <f>_xll.BDH(B$4,"PX_LAST",$B1,$B2,"Dir=V","Per=W","Dts=S","cols=2;rows=9")</f>
         <v>43931</v>
       </c>
       <c r="B5">
@@ -79816,7 +79887,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B13">
+        <v>851.98299999999995</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>

</xml_diff>